<commit_message>
added other functions by Rahul
</commit_message>
<xml_diff>
--- a/NHAI Data (1).xlsx
+++ b/NHAI Data (1).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>Chainage</t>
   </si>
@@ -55,6 +55,15 @@
     <t>Soil Types</t>
   </si>
   <si>
+    <t>Service Road Name</t>
+  </si>
+  <si>
+    <t>Service Road Side</t>
+  </si>
+  <si>
+    <t>Service Road Width</t>
+  </si>
+  <si>
     <t>Pond</t>
   </si>
   <si>
@@ -64,12 +73,21 @@
     <t>LHS</t>
   </si>
   <si>
+    <t>Hard</t>
+  </si>
+  <si>
     <t>Dhaba</t>
   </si>
   <si>
+    <t>Soft</t>
+  </si>
+  <si>
     <t>Farm</t>
   </si>
   <si>
+    <t>Normal</t>
+  </si>
+  <si>
     <t>Forest</t>
   </si>
   <si>
@@ -79,10 +97,10 @@
     <t>Shop</t>
   </si>
   <si>
+    <t>RHS</t>
+  </si>
+  <si>
     <t>Hotel</t>
-  </si>
-  <si>
-    <t>RHS</t>
   </si>
 </sst>
 </file>
@@ -380,6 +398,9 @@
     <col customWidth="1" min="8" max="8" width="27.0"/>
     <col customWidth="1" min="9" max="9" width="27.25"/>
     <col customWidth="1" min="14" max="14" width="14.13"/>
+    <col customWidth="1" min="15" max="15" width="16.5"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -425,7 +446,15 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
@@ -450,19 +479,23 @@
         <v>8.5</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="3">
@@ -487,15 +520,25 @@
         <v>8.5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3">
@@ -520,17 +563,21 @@
         <v>8.5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="3">
@@ -555,17 +602,21 @@
         <v>8.5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="N5" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -590,18 +641,23 @@
         <v>8.5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="N6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="3">
@@ -626,14 +682,25 @@
         <v>8.5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="N7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
@@ -658,16 +725,21 @@
         <v>8.5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="3">
@@ -692,16 +764,21 @@
         <v>8.5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="N9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="3">
@@ -726,16 +803,21 @@
         <v>8.5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="3">
@@ -760,18 +842,23 @@
         <v>8.5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="N11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="3">
@@ -796,14 +883,25 @@
         <v>8.5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="N12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3">
@@ -828,16 +926,21 @@
         <v>8.5</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="3">
@@ -862,16 +965,21 @@
         <v>8.5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="N14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="3">
@@ -901,7 +1009,18 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3">
@@ -926,16 +1045,21 @@
         <v>8.5</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="N16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="3">
@@ -960,20 +1084,25 @@
         <v>8.5</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L17" s="4">
         <v>22.0</v>
       </c>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="N17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="3">
@@ -998,14 +1127,19 @@
         <v>8.5</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="N18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="3">
@@ -1030,16 +1164,21 @@
         <v>8.5</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N19" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="3">
@@ -1069,8 +1208,12 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="4"/>
+      <c r="N20" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="3">
@@ -1095,17 +1238,27 @@
         <v>8.5</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="N21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>3.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>